<commit_message>
- updated command to use `profile` for configuring mail connectivity. - updated nexial's internal email notification code - cleaned up unused constants in NexialConst
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10422"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/showcase/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E75122F-2392-BF45-B088-D6C8E4370DC2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="20560" windowWidth="33600" xWindow="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440"/>
+    <workbookView xWindow="7360" yWindow="440" windowWidth="33600" windowHeight="20560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="#default" r:id="rId1" sheetId="2"/>
-    <sheet name="sentry_function_projectfile" r:id="rId2" sheetId="3"/>
-    <sheet name="crypto" r:id="rId3" sheetId="4"/>
-    <sheet name="repeat-test" r:id="rId4" sheetId="5"/>
-    <sheet name="expression-test" r:id="rId5" sheetId="6"/>
-    <sheet name="multi-scenario1" r:id="rId6" sheetId="7"/>
-    <sheet name="multi-scenario2" r:id="rId7" sheetId="8"/>
+    <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="nexial_function_projectfile" sheetId="3" r:id="rId2"/>
+    <sheet name="crypto" sheetId="4" r:id="rId3"/>
+    <sheet name="repeat-test" sheetId="5" r:id="rId4"/>
+    <sheet name="expression-test" sheetId="6" r:id="rId5"/>
+    <sheet name="multi-scenario1" sheetId="7" r:id="rId6"/>
+    <sheet name="multi-scenario2" sheetId="8" r:id="rId7"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId8"/>
@@ -46,7 +47,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -59,18 +60,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>sentry.pollWaitMs</t>
-  </si>
-  <si>
     <t>800</t>
-  </si>
-  <si>
-    <t>sentry.textDelim</t>
   </si>
   <si>
     <t>,</t>
@@ -82,31 +77,10 @@
     <t>var2</t>
   </si>
   <si>
-    <t>sentry.scope.mailTo</t>
-  </si>
-  <si>
-    <t>sentry.scope.executionMode</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
-    <t>sentry.scope.iteration</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>sentry.scope.fallbackToPrevious</t>
-  </si>
-  <si>
-    <t>sentry.delayBetweenStepsMs</t>
-  </si>
-  <si>
-    <t>sentry.failFast</t>
-  </si>
-  <si>
-    <t>sentry.verbose</t>
   </si>
   <si>
     <t>false</t>
@@ -178,9 +152,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>sentry.elapsedTimeSLA</t>
-  </si>
-  <si>
     <t>6000</t>
   </si>
   <si>
@@ -190,13 +161,7 @@
     <t>secretJane</t>
   </si>
   <si>
-    <t>crypt:4beafb332b5165ae0c6824feda3e88b80ab1a8fa5975ce63</t>
-  </si>
-  <si>
     <t>Cowabanga</t>
-  </si>
-  <si>
-    <t>sentry.scriptRef.startDate</t>
   </si>
   <si>
     <t>${startYear}-${startMonth}-${startDate}</t>
@@ -293,8 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="23">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -369,84 +333,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="26">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,127 +359,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -629,311 +398,81 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="3" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="9" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="4" fontId="10" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="18" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="6"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="8"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="10"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="9"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="11"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="132">
     <dxf>
@@ -2745,7 +2284,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2764,7 +2303,7 @@
       <sheetName val="#system"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData refreshError="1" sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2775,10 +2314,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2813,7 +2352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -2848,7 +2387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -2942,21 +2481,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2973,7 +2512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3025,35 +2564,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAB22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -3758,7 +3295,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4467,10 +4004,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -5176,7 +4713,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
@@ -5883,10 +5420,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -6592,10 +6129,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -7301,10 +6838,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -8010,10 +7547,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -8719,10 +8256,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -9428,10 +8965,10 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -10137,10 +9674,10 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -10846,14 +10383,14 @@
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -11556,16 +11093,16 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -12268,16 +11805,16 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -12980,16 +12517,16 @@
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -13692,13 +13229,13 @@
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -14400,15 +13937,15 @@
       <c r="ZY16"/>
       <c r="ZZ16"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:702">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -15110,15 +14647,15 @@
       <c r="ZY17"/>
       <c r="ZZ17"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:702">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -15820,12 +15357,12 @@
       <c r="ZY18"/>
       <c r="ZZ18"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:702">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -16528,12 +16065,12 @@
       <c r="ZY19"/>
       <c r="ZZ19"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:702">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -17236,12 +16773,12 @@
       <c r="ZY20"/>
       <c r="ZZ20"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:702">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -17944,12 +17481,12 @@
       <c r="ZY21"/>
       <c r="ZZ21"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:702">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
@@ -18653,130 +18190,130 @@
       <c r="ZZ22"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule dxfId="131" operator="beginsWith" priority="20" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="131" priority="20" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="130" operator="beginsWith" priority="21" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="130" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="129" priority="22" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="129" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule dxfId="128" priority="23" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="128" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="127" priority="24" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="127" priority="24">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule dxfId="126" priority="18" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="125" priority="19" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="125" priority="19">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule dxfId="124" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="123" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="123" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="122" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="122" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="121" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="121" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="120" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="120" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="119" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="119" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="118" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="118" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="117" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="116" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="116" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="115" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="114" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="114" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="113" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="112" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="112" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="111" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AAB14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AAA14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="24.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="24.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -19481,10 +19018,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -20190,10 +19727,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -20940,115 +20477,115 @@
       <c r="B14" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule dxfId="110" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="110" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="109" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="109" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="108" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="108" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule dxfId="107" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="107" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="106" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule dxfId="105" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="105" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="104" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="104" priority="16">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule dxfId="103" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="103" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="102" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="102" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="101" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="101" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="100" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="99" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="99" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="98" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="97" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="97" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="96" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="95" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="95" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="94" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="94" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="93" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="93" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="92" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="91" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="91" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="90" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AAB13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AAA13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -21757,10 +21294,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -22466,7 +22003,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -23173,10 +22710,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -23882,10 +23419,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -24591,10 +24128,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -25300,10 +24837,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -26009,7 +25546,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -26718,10 +26255,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -27439,115 +26976,115 @@
       <c r="B13" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A22:A1048576 A1:A18">
-    <cfRule dxfId="89" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="89" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="88" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="88" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="87" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B1048576 B1:B10">
-    <cfRule dxfId="86" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="86" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="85" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule dxfId="84" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="84" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="83" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="82" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="82" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="81" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="14">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="80" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="79" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="12">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="78" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="78" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="77" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="10">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="76" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="76" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="75" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="8">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="74" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="74" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="73" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="6">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="72" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="72" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="71" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="4">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="70" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="70" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="69" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="2">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AAB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -28256,10 +27793,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -28965,10 +28502,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -29674,10 +29211,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -30383,10 +29920,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -31092,10 +30629,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -31801,10 +31338,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -32526,118 +32063,118 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A17">
-    <cfRule dxfId="68" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="68" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="67" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="67" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="66" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule dxfId="65" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="65" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="64" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule dxfId="63" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="63" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="62" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="61" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="61" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="60" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="59" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="59" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="58" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="57" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="57" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="56" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="55" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="55" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="54" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="53" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="52" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="51" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="51" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="50" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="49" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="49" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="48" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AAB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -33343,10 +32880,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -34052,10 +33589,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -34761,10 +34298,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -35470,10 +35007,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -36179,7 +35716,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -36908,140 +36445,140 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A4 A7:A17">
-    <cfRule dxfId="47" operator="beginsWith" priority="23" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="47" priority="23" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="46" operator="beginsWith" priority="24" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="46" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="45" priority="25" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="25" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule dxfId="44" priority="26" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="44" priority="26" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="43" priority="27" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="27">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule dxfId="42" priority="21" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="42" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="41" priority="22" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="22">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="40" priority="19" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="40" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="39" priority="20" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="20">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="38" priority="17" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="38" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="37" priority="18" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="18">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="36" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="36" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="35" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="34" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="33" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="14">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="32" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="32" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="31" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="30" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="29" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="10">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="28" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="27" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule dxfId="26" operator="beginsWith" priority="4" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="26" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="25" operator="beginsWith" priority="5" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="25" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="24" priority="6" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule dxfId="23" operator="beginsWith" priority="1" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="22" operator="beginsWith" priority="2" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="21" priority="3" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AAB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -37747,10 +37284,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -38456,10 +37993,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -39165,10 +38702,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -39874,10 +39411,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -40583,7 +40120,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="11" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -41312,91 +40849,91 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A7:A17">
-    <cfRule dxfId="20" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="20" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="19" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="19" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="18" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B5:B9">
-    <cfRule dxfId="17" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="16" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="21">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule dxfId="15" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="14" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="13" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="12" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="11" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="10" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="9" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="8" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="7" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="6" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="5" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="4" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="3" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="2" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="1" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#### General - update execution output with different style/color for different columns - update execution output so that key columns are allocated sufficient width. - update execution output so that each row would be allocated sufficient height without appearing too "cramped". - update execution output so that "description" columns of macro, section and repeat-until will appear differently to provide better visual cues.
#### [base commands](../commands/base/index)
- [base &raquo; `macro(file,sheet,name)`](../commands/base/macro(file,sheet,name)) now merge with
  [base &raquo; `section(steps)`](../commands/base/section(steps)) so that we can express additional flow control
  nuances.
- [base &raquo; `section(steps)`](../commands/base/section(steps)): **NEW** command to capture macro steps so that
  flow control can be expressed across the entire "macro step group" (or section), or individually per step.

- remove dead code

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10422"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F091D59-4B6A-8948-82F8-8250D41F7170}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203B2E86-97B2-F647-9E24-40A95EBFB8D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="-20560" windowWidth="33600" windowHeight="10280" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -48,10 +48,15 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2870,7 +2875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -4303,7 +4310,7 @@
         <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -41238,9 +41245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE757796-35D5-EA4C-BA4E-99BB69CE7DE5}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>

</xml_diff>

<commit_message>
fixed output format issue, esp. dealing with description cells for macro/section and repeat-until
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203B2E86-97B2-F647-9E24-40A95EBFB8D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B324F7-3B58-8D44-93CB-0A38DAD4B2A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31540" yWindow="-20560" windowWidth="11200" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
### Flow Control - `TimeTrackStart(label)` and `TimeTrackEnd()`: new flow control to mark start/end time of any arbitrary group of steps.
#### Event Notification
- new event handling to mark the elapsed time of a well-defined events:
  - `nexial.trackExecution=true`: log start/end and elapsed time of an execution.
  - `nexial.trackScript=true`: log start/end and elapsed time of a script.
  - `nexial.trackIteration=true`: log start/end and elapsed time of an iteration.
  - `nexial.trackScenario=true`: log start/end and elapsed time of a scenario.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B324F7-3B58-8D44-93CB-0A38DAD4B2A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF520B2-B57A-7845-81DD-EAE477CC2E90}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31540" yWindow="-20560" windowWidth="11200" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26060" yWindow="-20560" windowWidth="16800" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -53,11 +53,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -66,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>true</t>
   </si>
@@ -258,6 +253,18 @@
   </si>
   <si>
     <t>nexial.scriptRef.startDate</t>
+  </si>
+  <si>
+    <t>nexial.trackExecution</t>
+  </si>
+  <si>
+    <t>nexial.trackScript</t>
+  </si>
+  <si>
+    <t>nexial.trackIteration</t>
+  </si>
+  <si>
+    <t>nexial.trackScenario</t>
   </si>
 </sst>
 </file>
@@ -2873,7 +2880,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA22"/>
+  <dimension ref="A1:AAA26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -18492,6 +18499,38 @@
       <c r="ZY22"/>
       <c r="ZZ22"/>
     </row>
+    <row r="23" spans="1:702">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:702">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:702">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:702">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
@@ -20874,7 +20913,7 @@
   <dimension ref="A1:AAA13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -27373,7 +27412,7 @@
   <dimension ref="A1:AAA12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>

<commit_message>
[io] - [`base64(var,file)`]: read and encode file content as base64.
[ws]
- [`upload(url,body,fileParams,var)`]: **NEW** command to upload one or
  more files as multipart-data, along with other request parameters, to specified endpoint (`url`).

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF520B2-B57A-7845-81DD-EAE477CC2E90}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC8AE0B-AB52-EF45-9EA9-CAAC494CC70F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26060" yWindow="-20560" windowWidth="16800" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="1080" windowWidth="16800" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>true</t>
   </si>
@@ -255,23 +255,35 @@
     <t>nexial.scriptRef.startDate</t>
   </si>
   <si>
-    <t>nexial.trackExecution</t>
+    <t>mliu@ep.com</t>
   </si>
   <si>
-    <t>nexial.trackScript</t>
+    <t>nexial.enableEmail</t>
   </si>
   <si>
-    <t>nexial.trackIteration</t>
+    <t>nexial.timetrack.trackExecution</t>
   </si>
   <si>
-    <t>nexial.trackScenario</t>
+    <t>nexial.timetrack.trackScript</t>
+  </si>
+  <si>
+    <t>nexial.timetrack.trackIteration</t>
+  </si>
+  <si>
+    <t>nexial.timetrack.trackScenario</t>
+  </si>
+  <si>
+    <t>nexial.notifyOnExecutionComplete</t>
+  </si>
+  <si>
+    <t>email:mliu@ep.com|Scenario $(execution|scenario|name) of $(execution|script|name) has started.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +358,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -373,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -411,6 +430,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -428,7 +458,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -476,6 +506,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -493,7 +531,72 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="158">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2880,10 +2983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA26"/>
+  <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -5025,7 +5128,9 @@
       <c r="A4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
@@ -18500,8 +18605,8 @@
       <c r="ZZ22"/>
     </row>
     <row r="23" spans="1:702">
-      <c r="A23" s="1" t="s">
-        <v>64</v>
+      <c r="A23" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>0</v>
@@ -18509,7 +18614,7 @@
     </row>
     <row r="24" spans="1:702">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
@@ -18517,7 +18622,7 @@
     </row>
     <row r="25" spans="1:702">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>0</v>
@@ -18525,97 +18630,135 @@
     </row>
     <row r="26" spans="1:702">
       <c r="A26" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="27" spans="1:702">
+      <c r="A27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:702">
+      <c r="A28" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule type="beginsWith" dxfId="152" priority="20" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+  <conditionalFormatting sqref="A23:A27 A1:A19 A29:A1048576">
+    <cfRule type="beginsWith" dxfId="157" priority="25" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="151" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="156" priority="26" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="150" priority="22" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="155" priority="27" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule type="expression" dxfId="149" priority="23" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B11 B15:B27 B29:B1048576">
+    <cfRule type="expression" dxfId="154" priority="28" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="148" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="153" priority="29">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="147" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="146" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="151" priority="24">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="145" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="144" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="149" priority="19">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="143" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="16" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="142" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="147" priority="17">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="141" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="140" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="145" priority="15">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="139" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="138" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="143" priority="13">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="137" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="10" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="136" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="141" priority="11">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="135" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="134" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="139" priority="9">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="133" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="6" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="132" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="137" priority="7">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A28,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A28,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(B28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{966ADFEE-6B36-8E45-A766-307055CBA106}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -20821,85 +20964,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule type="beginsWith" dxfId="131" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="136" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="135" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="129" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="134" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule type="expression" dxfId="128" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="127" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="132" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="125" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="130" priority="16">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="123" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="128" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="122" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="121" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="126" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="120" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="119" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="124" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="118" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="117" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="122" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="116" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="115" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="120" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="114" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="113" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="118" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="112" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="111" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="116" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27320,85 +27463,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A22:A1048576 A1:A18">
-    <cfRule type="beginsWith" dxfId="110" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="115" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="109" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="114" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="108" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B1048576 B1:B10">
-    <cfRule type="expression" dxfId="107" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="106" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="expression" dxfId="105" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="104" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="109" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="103" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="102" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="14">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="101" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="100" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="105" priority="12">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="99" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="98" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="103" priority="10">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="97" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="96" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="101" priority="8">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="95" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="94" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="99" priority="6">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="93" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="92" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="4">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="91" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="2">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32407,85 +32550,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A17">
-    <cfRule type="beginsWith" dxfId="89" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="94" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="93" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="87" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule type="expression" dxfId="86" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="84" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="83" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="82" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="81" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="79" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="78" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="77" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="76" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="74" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="73" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="72" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="71" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="70" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="69" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="74" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36789,107 +36932,107 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A4 A7:A17">
-    <cfRule type="beginsWith" dxfId="68" priority="23" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="73" priority="23" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="67" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="72" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="66" priority="25" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="25" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule type="expression" dxfId="65" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="26" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="64" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="27">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="63" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="62" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="22">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="61" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="20">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="59" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="58" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="18">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="57" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="56" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="55" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="54" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="14">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="53" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="52" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="51" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="10">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="beginsWith" dxfId="47" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="52" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="51" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="beginsWith" dxfId="44" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="43" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41193,85 +41336,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A7:A17">
-    <cfRule type="beginsWith" dxfId="41" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="46" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="45" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="39" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B5:B9">
-    <cfRule type="expression" dxfId="38" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="37" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="21">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="36" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="32" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="31" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="29" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="27" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="26" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="24" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56748,85 +56891,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule type="beginsWith" dxfId="20" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="25" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="24" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:B1048576 B1:B11">
-    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="16" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="16">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- further optimization of Nexial internal processing for faster startup time. - further improvement on Nexial Interactive, nearly 92% feature complete.   - added color output on console for Nexial Interactive; more to come.
[System Variable]
- [`nexial.var.defaultAsIs`] - **NEW** System variable to control unresolved data variable during substitution.

[web]
- [`openIgnoreTimeout`](../commands/web/openIngoreTimeout(url)): **NEW** command to open to a URL and tolerate page
  load that might extent between defined timeout (i.e. [`nexial.web.pageLoadWaitMs`]).

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11104"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC8AE0B-AB52-EF45-9EA9-CAAC494CC70F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE71299A-4F69-014D-94EE-732C3DFA1CB2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1080" windowWidth="16800" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25800" yWindow="16440" windowWidth="25400" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>true</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>var2</t>
-  </si>
-  <si>
-    <t>local</t>
   </si>
   <si>
     <t>1</t>
@@ -220,9 +217,6 @@
   </si>
   <si>
     <t>${user.name}</t>
-  </si>
-  <si>
-    <t>nexial.scope.executionMode</t>
   </si>
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
@@ -532,71 +526,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="158">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2435,6 +2364,71 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2983,10 +2977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA28"/>
+  <dimension ref="A1:AAA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -3000,10 +2994,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -3211,7 +3205,7 @@
       <c r="GX1"/>
       <c r="GY1"/>
       <c r="GZ1"/>
-      <c r="HA1"/>
+      <c r="HA1" s="7"/>
       <c r="HB1"/>
       <c r="HC1"/>
       <c r="HD1"/>
@@ -3705,13 +3699,14 @@
       <c r="ZX1"/>
       <c r="ZY1"/>
       <c r="ZZ1"/>
+      <c r="AAA1" s="7"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -4416,11 +4411,11 @@
       <c r="AAA2" s="7"/>
     </row>
     <row r="3" spans="1:703">
-      <c r="A3" s="1" t="s">
-        <v>55</v>
+      <c r="A3" s="6" t="s">
+        <v>54</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+      <c r="B3" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -5125,11 +5120,11 @@
       <c r="AAA3" s="7"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="6" t="s">
-        <v>56</v>
+      <c r="A4" s="1" t="s">
+        <v>55</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>64</v>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -5337,7 +5332,7 @@
       <c r="GX4"/>
       <c r="GY4"/>
       <c r="GZ4"/>
-      <c r="HA4" s="7"/>
+      <c r="HA4" s="4"/>
       <c r="HB4"/>
       <c r="HC4"/>
       <c r="HD4"/>
@@ -5831,14 +5826,14 @@
       <c r="ZX4"/>
       <c r="ZY4"/>
       <c r="ZZ4"/>
-      <c r="AAA4" s="7"/>
+      <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -6544,10 +6539,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -7253,10 +7248,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -7962,10 +7957,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -8671,7 +8666,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -9380,7 +9375,7 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -10089,13 +10084,15 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
+      <c r="B11" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C11"/>
-      <c r="D11"/>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
@@ -10300,7 +10297,7 @@
       <c r="GX11"/>
       <c r="GY11"/>
       <c r="GZ11"/>
-      <c r="HA11" s="4"/>
+      <c r="HA11"/>
       <c r="HB11"/>
       <c r="HC11"/>
       <c r="HD11"/>
@@ -10794,18 +10791,19 @@
       <c r="ZX11"/>
       <c r="ZY11"/>
       <c r="ZZ11"/>
-      <c r="AAA11" s="5"/>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
-      <c r="C12"/>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -11508,16 +11506,16 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -12220,16 +12218,16 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -12932,17 +12930,15 @@
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
@@ -13647,10 +13643,10 @@
         <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -14360,7 +14356,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -15064,14 +15060,12 @@
     </row>
     <row r="18" spans="1:702">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -15774,10 +15768,10 @@
     </row>
     <row r="19" spans="1:702">
       <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -16482,10 +16476,10 @@
     </row>
     <row r="20" spans="1:702">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -17190,10 +17184,10 @@
     </row>
     <row r="21" spans="1:702">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -17897,716 +17891,16 @@
       <c r="ZZ21"/>
     </row>
     <row r="22" spans="1:702">
-      <c r="A22" s="1" t="s">
-        <v>51</v>
+      <c r="A22" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
-      <c r="U22"/>
-      <c r="V22"/>
-      <c r="W22"/>
-      <c r="X22"/>
-      <c r="Y22"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-      <c r="AB22"/>
-      <c r="AC22"/>
-      <c r="AD22"/>
-      <c r="AE22"/>
-      <c r="AF22"/>
-      <c r="AG22"/>
-      <c r="AH22"/>
-      <c r="AI22"/>
-      <c r="AJ22"/>
-      <c r="AK22"/>
-      <c r="AL22"/>
-      <c r="AM22"/>
-      <c r="AN22"/>
-      <c r="AO22"/>
-      <c r="AP22"/>
-      <c r="AQ22"/>
-      <c r="AR22"/>
-      <c r="AS22"/>
-      <c r="AT22"/>
-      <c r="AU22"/>
-      <c r="AV22"/>
-      <c r="AW22"/>
-      <c r="AX22"/>
-      <c r="AY22"/>
-      <c r="AZ22"/>
-      <c r="BA22"/>
-      <c r="BB22"/>
-      <c r="BC22"/>
-      <c r="BD22"/>
-      <c r="BE22"/>
-      <c r="BF22"/>
-      <c r="BG22"/>
-      <c r="BH22"/>
-      <c r="BI22"/>
-      <c r="BJ22"/>
-      <c r="BK22"/>
-      <c r="BL22"/>
-      <c r="BM22"/>
-      <c r="BN22"/>
-      <c r="BO22"/>
-      <c r="BP22"/>
-      <c r="BQ22"/>
-      <c r="BR22"/>
-      <c r="BS22"/>
-      <c r="BT22"/>
-      <c r="BU22"/>
-      <c r="BV22"/>
-      <c r="BW22"/>
-      <c r="BX22"/>
-      <c r="BY22"/>
-      <c r="BZ22"/>
-      <c r="CA22"/>
-      <c r="CB22"/>
-      <c r="CC22"/>
-      <c r="CD22"/>
-      <c r="CE22"/>
-      <c r="CF22"/>
-      <c r="CG22"/>
-      <c r="CH22"/>
-      <c r="CI22"/>
-      <c r="CJ22"/>
-      <c r="CK22"/>
-      <c r="CL22"/>
-      <c r="CM22"/>
-      <c r="CN22"/>
-      <c r="CO22"/>
-      <c r="CP22"/>
-      <c r="CQ22"/>
-      <c r="CR22"/>
-      <c r="CS22"/>
-      <c r="CT22"/>
-      <c r="CU22"/>
-      <c r="CV22"/>
-      <c r="CW22"/>
-      <c r="CX22"/>
-      <c r="CY22"/>
-      <c r="CZ22"/>
-      <c r="DA22"/>
-      <c r="DB22"/>
-      <c r="DC22"/>
-      <c r="DD22"/>
-      <c r="DE22"/>
-      <c r="DF22"/>
-      <c r="DG22"/>
-      <c r="DH22"/>
-      <c r="DI22"/>
-      <c r="DJ22"/>
-      <c r="DK22"/>
-      <c r="DL22"/>
-      <c r="DM22"/>
-      <c r="DN22"/>
-      <c r="DO22"/>
-      <c r="DP22"/>
-      <c r="DQ22"/>
-      <c r="DR22"/>
-      <c r="DS22"/>
-      <c r="DT22"/>
-      <c r="DU22"/>
-      <c r="DV22"/>
-      <c r="DW22"/>
-      <c r="DX22"/>
-      <c r="DY22"/>
-      <c r="DZ22"/>
-      <c r="EA22"/>
-      <c r="EB22"/>
-      <c r="EC22"/>
-      <c r="ED22"/>
-      <c r="EE22"/>
-      <c r="EF22"/>
-      <c r="EG22"/>
-      <c r="EH22"/>
-      <c r="EI22"/>
-      <c r="EJ22"/>
-      <c r="EK22"/>
-      <c r="EL22"/>
-      <c r="EM22"/>
-      <c r="EN22"/>
-      <c r="EO22"/>
-      <c r="EP22"/>
-      <c r="EQ22"/>
-      <c r="ER22"/>
-      <c r="ES22"/>
-      <c r="ET22"/>
-      <c r="EU22"/>
-      <c r="EV22"/>
-      <c r="EW22"/>
-      <c r="EX22"/>
-      <c r="EY22"/>
-      <c r="EZ22"/>
-      <c r="FA22"/>
-      <c r="FB22"/>
-      <c r="FC22"/>
-      <c r="FD22"/>
-      <c r="FE22"/>
-      <c r="FF22"/>
-      <c r="FG22"/>
-      <c r="FH22"/>
-      <c r="FI22"/>
-      <c r="FJ22"/>
-      <c r="FK22"/>
-      <c r="FL22"/>
-      <c r="FM22"/>
-      <c r="FN22"/>
-      <c r="FO22"/>
-      <c r="FP22"/>
-      <c r="FQ22"/>
-      <c r="FR22"/>
-      <c r="FS22"/>
-      <c r="FT22"/>
-      <c r="FU22"/>
-      <c r="FV22"/>
-      <c r="FW22"/>
-      <c r="FX22"/>
-      <c r="FY22"/>
-      <c r="FZ22"/>
-      <c r="GA22"/>
-      <c r="GB22"/>
-      <c r="GC22"/>
-      <c r="GD22"/>
-      <c r="GE22"/>
-      <c r="GF22"/>
-      <c r="GG22"/>
-      <c r="GH22"/>
-      <c r="GI22"/>
-      <c r="GJ22"/>
-      <c r="GK22"/>
-      <c r="GL22"/>
-      <c r="GM22"/>
-      <c r="GN22"/>
-      <c r="GO22"/>
-      <c r="GP22"/>
-      <c r="GQ22"/>
-      <c r="GR22"/>
-      <c r="GS22"/>
-      <c r="GT22"/>
-      <c r="GU22"/>
-      <c r="GV22"/>
-      <c r="GW22"/>
-      <c r="GX22"/>
-      <c r="GY22"/>
-      <c r="GZ22"/>
-      <c r="HA22"/>
-      <c r="HB22"/>
-      <c r="HC22"/>
-      <c r="HD22"/>
-      <c r="HE22"/>
-      <c r="HF22"/>
-      <c r="HG22"/>
-      <c r="HH22"/>
-      <c r="HI22"/>
-      <c r="HJ22"/>
-      <c r="HK22"/>
-      <c r="HL22"/>
-      <c r="HM22"/>
-      <c r="HN22"/>
-      <c r="HO22"/>
-      <c r="HP22"/>
-      <c r="HQ22"/>
-      <c r="HR22"/>
-      <c r="HS22"/>
-      <c r="HT22"/>
-      <c r="HU22"/>
-      <c r="HV22"/>
-      <c r="HW22"/>
-      <c r="HX22"/>
-      <c r="HY22"/>
-      <c r="HZ22"/>
-      <c r="IA22"/>
-      <c r="IB22"/>
-      <c r="IC22"/>
-      <c r="ID22"/>
-      <c r="IE22"/>
-      <c r="IF22"/>
-      <c r="IG22"/>
-      <c r="IH22"/>
-      <c r="II22"/>
-      <c r="IJ22"/>
-      <c r="IK22"/>
-      <c r="IL22"/>
-      <c r="IM22"/>
-      <c r="IN22"/>
-      <c r="IO22"/>
-      <c r="IP22"/>
-      <c r="IQ22"/>
-      <c r="IR22"/>
-      <c r="IS22"/>
-      <c r="IT22"/>
-      <c r="IU22"/>
-      <c r="IV22"/>
-      <c r="IW22"/>
-      <c r="IX22"/>
-      <c r="IY22"/>
-      <c r="IZ22"/>
-      <c r="JA22"/>
-      <c r="JB22"/>
-      <c r="JC22"/>
-      <c r="JD22"/>
-      <c r="JE22"/>
-      <c r="JF22"/>
-      <c r="JG22"/>
-      <c r="JH22"/>
-      <c r="JI22"/>
-      <c r="JJ22"/>
-      <c r="JK22"/>
-      <c r="JL22"/>
-      <c r="JM22"/>
-      <c r="JN22"/>
-      <c r="JO22"/>
-      <c r="JP22"/>
-      <c r="JQ22"/>
-      <c r="JR22"/>
-      <c r="JS22"/>
-      <c r="JT22"/>
-      <c r="JU22"/>
-      <c r="JV22"/>
-      <c r="JW22"/>
-      <c r="JX22"/>
-      <c r="JY22"/>
-      <c r="JZ22"/>
-      <c r="KA22"/>
-      <c r="KB22"/>
-      <c r="KC22"/>
-      <c r="KD22"/>
-      <c r="KE22"/>
-      <c r="KF22"/>
-      <c r="KG22"/>
-      <c r="KH22"/>
-      <c r="KI22"/>
-      <c r="KJ22"/>
-      <c r="KK22"/>
-      <c r="KL22"/>
-      <c r="KM22"/>
-      <c r="KN22"/>
-      <c r="KO22"/>
-      <c r="KP22"/>
-      <c r="KQ22"/>
-      <c r="KR22"/>
-      <c r="KS22"/>
-      <c r="KT22"/>
-      <c r="KU22"/>
-      <c r="KV22"/>
-      <c r="KW22"/>
-      <c r="KX22"/>
-      <c r="KY22"/>
-      <c r="KZ22"/>
-      <c r="LA22"/>
-      <c r="LB22"/>
-      <c r="LC22"/>
-      <c r="LD22"/>
-      <c r="LE22"/>
-      <c r="LF22"/>
-      <c r="LG22"/>
-      <c r="LH22"/>
-      <c r="LI22"/>
-      <c r="LJ22"/>
-      <c r="LK22"/>
-      <c r="LL22"/>
-      <c r="LM22"/>
-      <c r="LN22"/>
-      <c r="LO22"/>
-      <c r="LP22"/>
-      <c r="LQ22"/>
-      <c r="LR22"/>
-      <c r="LS22"/>
-      <c r="LT22"/>
-      <c r="LU22"/>
-      <c r="LV22"/>
-      <c r="LW22"/>
-      <c r="LX22"/>
-      <c r="LY22"/>
-      <c r="LZ22"/>
-      <c r="MA22"/>
-      <c r="MB22"/>
-      <c r="MC22"/>
-      <c r="MD22"/>
-      <c r="ME22"/>
-      <c r="MF22"/>
-      <c r="MG22"/>
-      <c r="MH22"/>
-      <c r="MI22"/>
-      <c r="MJ22"/>
-      <c r="MK22"/>
-      <c r="ML22"/>
-      <c r="MM22"/>
-      <c r="MN22"/>
-      <c r="MO22"/>
-      <c r="MP22"/>
-      <c r="MQ22"/>
-      <c r="MR22"/>
-      <c r="MS22"/>
-      <c r="MT22"/>
-      <c r="MU22"/>
-      <c r="MV22"/>
-      <c r="MW22"/>
-      <c r="MX22"/>
-      <c r="MY22"/>
-      <c r="MZ22"/>
-      <c r="NA22"/>
-      <c r="NB22"/>
-      <c r="NC22"/>
-      <c r="ND22"/>
-      <c r="NE22"/>
-      <c r="NF22"/>
-      <c r="NG22"/>
-      <c r="NH22"/>
-      <c r="NI22"/>
-      <c r="NJ22"/>
-      <c r="NK22"/>
-      <c r="NL22"/>
-      <c r="NM22"/>
-      <c r="NN22"/>
-      <c r="NO22"/>
-      <c r="NP22"/>
-      <c r="NQ22"/>
-      <c r="NR22"/>
-      <c r="NS22"/>
-      <c r="NT22"/>
-      <c r="NU22"/>
-      <c r="NV22"/>
-      <c r="NW22"/>
-      <c r="NX22"/>
-      <c r="NY22"/>
-      <c r="NZ22"/>
-      <c r="OA22"/>
-      <c r="OB22"/>
-      <c r="OC22"/>
-      <c r="OD22"/>
-      <c r="OE22"/>
-      <c r="OF22"/>
-      <c r="OG22"/>
-      <c r="OH22"/>
-      <c r="OI22"/>
-      <c r="OJ22"/>
-      <c r="OK22"/>
-      <c r="OL22"/>
-      <c r="OM22"/>
-      <c r="ON22"/>
-      <c r="OO22"/>
-      <c r="OP22"/>
-      <c r="OQ22"/>
-      <c r="OR22"/>
-      <c r="OS22"/>
-      <c r="OT22"/>
-      <c r="OU22"/>
-      <c r="OV22"/>
-      <c r="OW22"/>
-      <c r="OX22"/>
-      <c r="OY22"/>
-      <c r="OZ22"/>
-      <c r="PA22"/>
-      <c r="PB22"/>
-      <c r="PC22"/>
-      <c r="PD22"/>
-      <c r="PE22"/>
-      <c r="PF22"/>
-      <c r="PG22"/>
-      <c r="PH22"/>
-      <c r="PI22"/>
-      <c r="PJ22"/>
-      <c r="PK22"/>
-      <c r="PL22"/>
-      <c r="PM22"/>
-      <c r="PN22"/>
-      <c r="PO22"/>
-      <c r="PP22"/>
-      <c r="PQ22"/>
-      <c r="PR22"/>
-      <c r="PS22"/>
-      <c r="PT22"/>
-      <c r="PU22"/>
-      <c r="PV22"/>
-      <c r="PW22"/>
-      <c r="PX22"/>
-      <c r="PY22"/>
-      <c r="PZ22"/>
-      <c r="QA22"/>
-      <c r="QB22"/>
-      <c r="QC22"/>
-      <c r="QD22"/>
-      <c r="QE22"/>
-      <c r="QF22"/>
-      <c r="QG22"/>
-      <c r="QH22"/>
-      <c r="QI22"/>
-      <c r="QJ22"/>
-      <c r="QK22"/>
-      <c r="QL22"/>
-      <c r="QM22"/>
-      <c r="QN22"/>
-      <c r="QO22"/>
-      <c r="QP22"/>
-      <c r="QQ22"/>
-      <c r="QR22"/>
-      <c r="QS22"/>
-      <c r="QT22"/>
-      <c r="QU22"/>
-      <c r="QV22"/>
-      <c r="QW22"/>
-      <c r="QX22"/>
-      <c r="QY22"/>
-      <c r="QZ22"/>
-      <c r="RA22"/>
-      <c r="RB22"/>
-      <c r="RC22"/>
-      <c r="RD22"/>
-      <c r="RE22"/>
-      <c r="RF22"/>
-      <c r="RG22"/>
-      <c r="RH22"/>
-      <c r="RI22"/>
-      <c r="RJ22"/>
-      <c r="RK22"/>
-      <c r="RL22"/>
-      <c r="RM22"/>
-      <c r="RN22"/>
-      <c r="RO22"/>
-      <c r="RP22"/>
-      <c r="RQ22"/>
-      <c r="RR22"/>
-      <c r="RS22"/>
-      <c r="RT22"/>
-      <c r="RU22"/>
-      <c r="RV22"/>
-      <c r="RW22"/>
-      <c r="RX22"/>
-      <c r="RY22"/>
-      <c r="RZ22"/>
-      <c r="SA22"/>
-      <c r="SB22"/>
-      <c r="SC22"/>
-      <c r="SD22"/>
-      <c r="SE22"/>
-      <c r="SF22"/>
-      <c r="SG22"/>
-      <c r="SH22"/>
-      <c r="SI22"/>
-      <c r="SJ22"/>
-      <c r="SK22"/>
-      <c r="SL22"/>
-      <c r="SM22"/>
-      <c r="SN22"/>
-      <c r="SO22"/>
-      <c r="SP22"/>
-      <c r="SQ22"/>
-      <c r="SR22"/>
-      <c r="SS22"/>
-      <c r="ST22"/>
-      <c r="SU22"/>
-      <c r="SV22"/>
-      <c r="SW22"/>
-      <c r="SX22"/>
-      <c r="SY22"/>
-      <c r="SZ22"/>
-      <c r="TA22"/>
-      <c r="TB22"/>
-      <c r="TC22"/>
-      <c r="TD22"/>
-      <c r="TE22"/>
-      <c r="TF22"/>
-      <c r="TG22"/>
-      <c r="TH22"/>
-      <c r="TI22"/>
-      <c r="TJ22"/>
-      <c r="TK22"/>
-      <c r="TL22"/>
-      <c r="TM22"/>
-      <c r="TN22"/>
-      <c r="TO22"/>
-      <c r="TP22"/>
-      <c r="TQ22"/>
-      <c r="TR22"/>
-      <c r="TS22"/>
-      <c r="TT22"/>
-      <c r="TU22"/>
-      <c r="TV22"/>
-      <c r="TW22"/>
-      <c r="TX22"/>
-      <c r="TY22"/>
-      <c r="TZ22"/>
-      <c r="UA22"/>
-      <c r="UB22"/>
-      <c r="UC22"/>
-      <c r="UD22"/>
-      <c r="UE22"/>
-      <c r="UF22"/>
-      <c r="UG22"/>
-      <c r="UH22"/>
-      <c r="UI22"/>
-      <c r="UJ22"/>
-      <c r="UK22"/>
-      <c r="UL22"/>
-      <c r="UM22"/>
-      <c r="UN22"/>
-      <c r="UO22"/>
-      <c r="UP22"/>
-      <c r="UQ22"/>
-      <c r="UR22"/>
-      <c r="US22"/>
-      <c r="UT22"/>
-      <c r="UU22"/>
-      <c r="UV22"/>
-      <c r="UW22"/>
-      <c r="UX22"/>
-      <c r="UY22"/>
-      <c r="UZ22"/>
-      <c r="VA22"/>
-      <c r="VB22"/>
-      <c r="VC22"/>
-      <c r="VD22"/>
-      <c r="VE22"/>
-      <c r="VF22"/>
-      <c r="VG22"/>
-      <c r="VH22"/>
-      <c r="VI22"/>
-      <c r="VJ22"/>
-      <c r="VK22"/>
-      <c r="VL22"/>
-      <c r="VM22"/>
-      <c r="VN22"/>
-      <c r="VO22"/>
-      <c r="VP22"/>
-      <c r="VQ22"/>
-      <c r="VR22"/>
-      <c r="VS22"/>
-      <c r="VT22"/>
-      <c r="VU22"/>
-      <c r="VV22"/>
-      <c r="VW22"/>
-      <c r="VX22"/>
-      <c r="VY22"/>
-      <c r="VZ22"/>
-      <c r="WA22"/>
-      <c r="WB22"/>
-      <c r="WC22"/>
-      <c r="WD22"/>
-      <c r="WE22"/>
-      <c r="WF22"/>
-      <c r="WG22"/>
-      <c r="WH22"/>
-      <c r="WI22"/>
-      <c r="WJ22"/>
-      <c r="WK22"/>
-      <c r="WL22"/>
-      <c r="WM22"/>
-      <c r="WN22"/>
-      <c r="WO22"/>
-      <c r="WP22"/>
-      <c r="WQ22"/>
-      <c r="WR22"/>
-      <c r="WS22"/>
-      <c r="WT22"/>
-      <c r="WU22"/>
-      <c r="WV22"/>
-      <c r="WW22"/>
-      <c r="WX22"/>
-      <c r="WY22"/>
-      <c r="WZ22"/>
-      <c r="XA22"/>
-      <c r="XB22"/>
-      <c r="XC22"/>
-      <c r="XD22"/>
-      <c r="XE22"/>
-      <c r="XF22"/>
-      <c r="XG22"/>
-      <c r="XH22"/>
-      <c r="XI22"/>
-      <c r="XJ22"/>
-      <c r="XK22"/>
-      <c r="XL22"/>
-      <c r="XM22"/>
-      <c r="XN22"/>
-      <c r="XO22"/>
-      <c r="XP22"/>
-      <c r="XQ22"/>
-      <c r="XR22"/>
-      <c r="XS22"/>
-      <c r="XT22"/>
-      <c r="XU22"/>
-      <c r="XV22"/>
-      <c r="XW22"/>
-      <c r="XX22"/>
-      <c r="XY22"/>
-      <c r="XZ22"/>
-      <c r="YA22"/>
-      <c r="YB22"/>
-      <c r="YC22"/>
-      <c r="YD22"/>
-      <c r="YE22"/>
-      <c r="YF22"/>
-      <c r="YG22"/>
-      <c r="YH22"/>
-      <c r="YI22"/>
-      <c r="YJ22"/>
-      <c r="YK22"/>
-      <c r="YL22"/>
-      <c r="YM22"/>
-      <c r="YN22"/>
-      <c r="YO22"/>
-      <c r="YP22"/>
-      <c r="YQ22"/>
-      <c r="YR22"/>
-      <c r="YS22"/>
-      <c r="YT22"/>
-      <c r="YU22"/>
-      <c r="YV22"/>
-      <c r="YW22"/>
-      <c r="YX22"/>
-      <c r="YY22"/>
-      <c r="YZ22"/>
-      <c r="ZA22"/>
-      <c r="ZB22"/>
-      <c r="ZC22"/>
-      <c r="ZD22"/>
-      <c r="ZE22"/>
-      <c r="ZF22"/>
-      <c r="ZG22"/>
-      <c r="ZH22"/>
-      <c r="ZI22"/>
-      <c r="ZJ22"/>
-      <c r="ZK22"/>
-      <c r="ZL22"/>
-      <c r="ZM22"/>
-      <c r="ZN22"/>
-      <c r="ZO22"/>
-      <c r="ZP22"/>
-      <c r="ZQ22"/>
-      <c r="ZR22"/>
-      <c r="ZS22"/>
-      <c r="ZT22"/>
-      <c r="ZU22"/>
-      <c r="ZV22"/>
-      <c r="ZW22"/>
-      <c r="ZX22"/>
-      <c r="ZY22"/>
-      <c r="ZZ22"/>
     </row>
     <row r="23" spans="1:702">
-      <c r="A23" s="6" t="s">
-        <v>66</v>
+      <c r="A23" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>0</v>
@@ -18614,7 +17908,7 @@
     </row>
     <row r="24" spans="1:702">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
@@ -18622,7 +17916,7 @@
     </row>
     <row r="25" spans="1:702">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>0</v>
@@ -18630,31 +17924,23 @@
     </row>
     <row r="26" spans="1:702">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:702">
-      <c r="A27" s="1" t="s">
-        <v>65</v>
+      <c r="A27" s="6" t="s">
+        <v>68</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:702">
-      <c r="A28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>71</v>
+      <c r="B27" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A23:A27 A1:A19 A29:A1048576">
+  <conditionalFormatting sqref="A22:A26 A28:A1048576 A1:A18">
     <cfRule type="beginsWith" dxfId="157" priority="25" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
@@ -18665,7 +17951,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B11 B15:B27 B29:B1048576">
+  <conditionalFormatting sqref="B14:B26 B28:B1048576 B1:B10">
     <cfRule type="expression" dxfId="154" priority="28" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
@@ -18673,91 +17959,91 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B14">
+  <conditionalFormatting sqref="B11:B13">
     <cfRule type="expression" dxfId="152" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="151" priority="24">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
+  <conditionalFormatting sqref="B13">
     <cfRule type="expression" dxfId="150" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="149" priority="19">
-      <formula>LEN(TRIM(B14))&gt;0</formula>
+      <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B12">
     <cfRule type="expression" dxfId="148" priority="16" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="147" priority="17">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
+      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B12">
     <cfRule type="expression" dxfId="146" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="145" priority="15">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
+      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="B11">
     <cfRule type="expression" dxfId="144" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="143" priority="13">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B12">
     <cfRule type="expression" dxfId="142" priority="10" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="141" priority="11">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
+      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="B11">
     <cfRule type="expression" dxfId="140" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="139" priority="9">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="B11">
     <cfRule type="expression" dxfId="138" priority="6" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="137" priority="7">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A28,LEN("sentry.scope."))="sentry.scope."</formula>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="beginsWith" dxfId="136" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A27,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A28,LEN("sentry."))="sentry."</formula>
+    <cfRule type="beginsWith" dxfId="135" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A27,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="134" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="133" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(B28))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="132" priority="5">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{966ADFEE-6B36-8E45-A766-307055CBA106}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{966ADFEE-6B36-8E45-A766-307055CBA106}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18795,10 +18081,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -19503,10 +18789,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -20212,10 +19498,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -20964,85 +20250,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule type="beginsWith" dxfId="136" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="131" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="135" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="130" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="134" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="129" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule type="expression" dxfId="133" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="132" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="127" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="131" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="130" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="125" priority="16">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="129" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="128" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="123" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="127" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="126" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="121" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="125" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="124" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="119" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="123" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="122" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="121" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="120" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="119" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="118" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="117" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="116" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21070,7 +20356,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -21779,10 +21065,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -22488,7 +21774,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -23195,10 +22481,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -23904,10 +23190,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -24613,7 +23899,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -25322,7 +24608,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -26031,7 +25317,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -26740,10 +26026,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -27463,85 +26749,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A22:A1048576 A1:A18">
-    <cfRule type="beginsWith" dxfId="115" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="110" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="114" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="109" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="113" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="108" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B1048576 B1:B10">
-    <cfRule type="expression" dxfId="112" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="111" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="expression" dxfId="110" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="109" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="104" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="108" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="107" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="102" priority="14">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="106" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="105" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="12">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="104" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="103" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="10">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="102" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="101" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="8">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="100" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="99" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="94" priority="6">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="98" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="97" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="4">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="96" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="2">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27569,7 +26855,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -28278,10 +27564,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -28987,10 +28273,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -29696,10 +28982,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -30405,7 +29691,7 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -31114,7 +30400,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -31823,10 +31109,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -32550,85 +31836,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A17">
-    <cfRule type="beginsWith" dxfId="94" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="89" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="93" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="88" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="92" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule type="expression" dxfId="91" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="89" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="88" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="87" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="86" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="85" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="84" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="83" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="82" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="81" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="79" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="78" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="77" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="76" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="75" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="74" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32656,10 +31942,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -33365,10 +32651,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -34074,10 +33360,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -34783,10 +34069,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -35492,10 +34778,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -36201,7 +35487,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -36932,107 +36218,107 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A4 A7:A17">
-    <cfRule type="beginsWith" dxfId="73" priority="23" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="68" priority="23" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="67" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="71" priority="25" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="25" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule type="expression" dxfId="70" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="26" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="69" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="27">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="67" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="22">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="66" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="20">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="64" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="63" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="18">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="62" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="61" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="60" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="59" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="14">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="58" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="57" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="56" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="10">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="54" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="beginsWith" dxfId="52" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="51" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="46" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="44" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="43" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37060,10 +36346,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -37769,10 +37055,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -38478,10 +37764,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -39187,10 +38473,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -39896,10 +39182,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -40605,7 +39891,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -41336,85 +40622,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A7:A17">
-    <cfRule type="beginsWith" dxfId="46" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="41" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="45" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="40" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="44" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B5:B9">
-    <cfRule type="expression" dxfId="43" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="21">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="41" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="39" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="37" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="36" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="34" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="33" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="32" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="29" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56891,85 +56177,85 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule type="beginsWith" dxfId="25" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="20" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="19" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="19" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:B1048576 B1:B11">
-    <cfRule type="expression" dxfId="22" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="20" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="19" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="16" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="11" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
### General - rename some System variables so that their name are prefixed with `nexial.` to avoid conflicts.
### [Nexial Interactive](../interactive)
- now supports reloading of `project.properties` (option: `9`)

### [image commands](../commands/image)
- [`compare(baseline,actual)`](../commands/image/compare(baseline,actual)): increase the thickness of the highlighting
  border to improve readability.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11104"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE71299A-4F69-014D-94EE-732C3DFA1CB2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D2AA02-1474-204D-9B79-74C20470E132}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="16440" windowWidth="25400" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,7 +270,7 @@
     <t>nexial.notifyOnExecutionComplete</t>
   </si>
   <si>
-    <t>email:mliu@ep.com|Scenario $(execution|scenario|name) of $(execution|script|name) has started.</t>
+    <t>email:mliu@ep.com|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
   </si>
 </sst>
 </file>
@@ -2980,7 +2980,7 @@
   <dimension ref="A1:AAA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>

<commit_message>
- fixed gmail mail support due to namespace conflict in mail configuration. - propagate changes between iterations. - add `[nexial] ` prefix to mail subject in mail notificaiton.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED0351A-FBEB-2F46-A83E-18CC83272E5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D422E294-C6C8-FC46-9E78-89438B932AA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="10060" windowWidth="25400" windowHeight="15500" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15560" yWindow="10060" windowWidth="25400" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>true</t>
   </si>
@@ -277,7 +277,13 @@
     <t>nexial.notifyOnExecutionComplete</t>
   </si>
   <si>
-    <t>email:mliu@ep.com|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
+    <t>nexial.mailTo</t>
+  </si>
+  <si>
+    <t>mike.liu.ep@gmail.com</t>
+  </si>
+  <si>
+    <t>email:mike.liu.ep@gmail.com|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
   </si>
 </sst>
 </file>
@@ -3564,7 +3570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -18520,7 +18526,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -18639,7 +18645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B44FF11-61AF-9941-8CEA-991BA6A370B6}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -72425,7 +72431,7 @@
   <dimension ref="A1:AAA22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -73855,7 +73861,12 @@
       <c r="AAA2" s="7"/>
     </row>
     <row r="3" spans="1:703">
-      <c r="B3" s="12"/>
+      <c r="A3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
@@ -87986,6 +87997,9 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CC5BD923-8B51-DE47-8D2D-7FA0104BF790}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
[Event Notification] - now supports conditional event notification via `nexial.notifyOn...If` data variables:
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D422E294-C6C8-FC46-9E78-89438B932AA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA4414E-A071-FE47-8A65-E6C3F56C628B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="10060" windowWidth="25400" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25180" yWindow="14180" windowWidth="25400" windowHeight="15500" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>true</t>
   </si>
@@ -284,6 +284,21 @@
   </si>
   <si>
     <t>email:mike.liu.ep@gmail.com|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
+  </si>
+  <si>
+    <t>nexial.notifyOnExecutionCompleteIf</t>
+  </si>
+  <si>
+    <t>1=2</t>
+  </si>
+  <si>
+    <t>nexial.notifyOnIterationComplete</t>
+  </si>
+  <si>
+    <t>nexial.notifyOnIterationCompleteIf</t>
+  </si>
+  <si>
+    <t>${nexial.scope.currentIteration}=2</t>
   </si>
 </sst>
 </file>
@@ -3568,10 +3583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA27"/>
+  <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -18527,6 +18542,14 @@
       </c>
       <c r="B27" s="14" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:702">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -72430,8 +72453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F7CABA-3882-0740-AF64-AD7DE14CE12E}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -73156,7 +73179,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -74570,7 +74593,12 @@
       <c r="AAA3" s="7"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
@@ -75274,6 +75302,12 @@
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>

</xml_diff>

<commit_message>
- minor code fix for `nexial-crypt` to accept input with spaces.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA4414E-A071-FE47-8A65-E6C3F56C628B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B546D26B-8A2D-C045-A924-83A66FEBA7F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25180" yWindow="14180" windowWidth="25400" windowHeight="15500" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25180" yWindow="14180" windowWidth="25400" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
   <si>
     <t>true</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t>${nexial.scope.currentIteration}=2</t>
+  </si>
+  <si>
+    <t>testdata1</t>
+  </si>
+  <si>
+    <t>testfile</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/jmeter-sample2.jmx</t>
+  </si>
+  <si>
+    <t>crypt:0d3086d52f3037a6403c2c6f3e8620755ff547fe550980fd654251f2d4f44b03</t>
   </si>
 </sst>
 </file>
@@ -34249,8 +34261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AAA14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -36389,11 +36401,22 @@
       <c r="AAA3" s="7"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="HA4" s="7"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
@@ -72453,7 +72476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F7CABA-3882-0740-AF64-AD7DE14CE12E}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- [`nexial-variable-update`] script now supports macro and HTML files. Also reduced excessive logging. - event notification: mail notification now supports HTML via System variable `nexial.notifyViaHTML`. - execution: better support for execution metadata, specifically for scenario and script
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B546D26B-8A2D-C045-A924-83A66FEBA7F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1062F4-CDFE-C34F-958C-C4216427B59F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25180" yWindow="14180" windowWidth="25400" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25180" yWindow="14180" windowWidth="25400" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>true</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>crypt:0d3086d52f3037a6403c2c6f3e8620755ff547fe550980fd654251f2d4f44b03</t>
+  </si>
+  <si>
+    <t>email:your_email_here|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
   </si>
 </sst>
 </file>
@@ -3597,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B28" sqref="A28:B28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -18553,7 +18556,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:702">
@@ -34261,7 +34264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AAA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[fixes] - if a hyperlink is too long to be contained in an Excel cell, Nexial will render it as plain text. Otherwise user might   get a runtime exception.
[improvements]
- enhanced to support the rendering of multi-line or wrapped text in execution output (Excel).

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F2EE48-9F8C-0142-AF9F-79B3ACD81109}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D54E627-9034-3947-BB47-F2FAD0A2582B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="89">
   <si>
     <t>true</t>
   </si>
@@ -228,12 +228,6 @@
     <t>1=2</t>
   </si>
   <si>
-    <t>nexial.mailSubject</t>
-  </si>
-  <si>
-    <t>nexial.mailHeader</t>
-  </si>
-  <si>
     <t>any question or inquiry, refer to &lt;a href="mailto:mliu@ep.com"&gt;Mike&lt;/a&gt;. Thanks!</t>
   </si>
   <si>
@@ -315,6 +309,12 @@
     <t>${nexial.scope.currentIteration}=2</t>
   </si>
   <si>
+    <t>// nexial.mailSubject</t>
+  </si>
+  <si>
+    <t>// nexial.mailHeader</t>
+  </si>
+  <si>
     <t>// nexial.mailFooter</t>
   </si>
   <si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Dummy Test, Please Ignore. Thanks!</t>
+  </si>
+  <si>
+    <t>mliu@ep.com,spopovic@ep.com</t>
   </si>
 </sst>
 </file>
@@ -19943,7 +19946,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -19959,7 +19962,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="HA1" s="3" t="s">
         <v>11</v>
@@ -19973,7 +19976,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="HA2" s="3" t="s">
         <v>11</v>
@@ -19984,7 +19987,7 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>86</v>
@@ -19998,7 +20001,7 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>87</v>
@@ -20015,7 +20018,7 @@
         <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="HA5" s="6" t="s">
         <v>11</v>
@@ -20683,10 +20686,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -21396,10 +21399,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -22822,10 +22825,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="HA4" s="6" t="s">
         <v>11</v>
@@ -22836,10 +22839,10 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="HA5" s="6" t="s">
         <v>11</v>
@@ -29207,10 +29210,10 @@
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -36155,10 +36158,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -36868,10 +36871,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -37581,10 +37584,10 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -38294,10 +38297,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -41076,10 +41079,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -41789,10 +41792,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -42502,10 +42505,10 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -43215,10 +43218,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -43931,7 +43934,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -46713,7 +46716,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -47426,7 +47429,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -48136,10 +48139,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -48849,10 +48852,10 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>

</xml_diff>

<commit_message>
- slight excel row height adjustments - set excel sheet to auto adjust cell width on activity, description and command
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D54E627-9034-3947-BB47-F2FAD0A2582B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5711C0BC-9E9E-E040-8831-5CFA1BE584C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19945,8 +19945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487F2C1F-1995-ED42-8C56-BA026F6A1911}">
   <dimension ref="A1:AAA200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[fixes] - Project Inspector:   - registered previously missed System variables for better project inspection; otherwise project inspector would report valid System variables as "unknown".   - fixed incorrect test step row number reported in project inspector HTML.
[rdbms]
- correctly capture rollback statements/events.
- replace deprecated DBCP API code
- forced single-query transaction to close connection after execution; required to avoid resource contention.

[web]
- browser metrics: fixed timing calculation to avoid negative time.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/base-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11103"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5711C0BC-9E9E-E040-8831-5CFA1BE584C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774D32E4-9054-5742-9C35-BF6E39D56D38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="38400" windowHeight="35540" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="4" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="88">
   <si>
     <t>true</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>nexial.mailTo</t>
-  </si>
-  <si>
-    <t>mliu@ep.com</t>
   </si>
   <si>
     <t>nexial.delayBetweenStepsMs</t>
@@ -294,13 +291,7 @@
     <t>1-2</t>
   </si>
   <si>
-    <t>mike.liu.ep@gmail.com</t>
-  </si>
-  <si>
     <t>nexial.notifyOnIterationComplete</t>
-  </si>
-  <si>
-    <t>email:mike.liu.ep@gmail.com|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
   </si>
   <si>
     <t>nexial.notifyOnIterationCompleteIf</t>
@@ -324,7 +315,13 @@
     <t>Dummy Test, Please Ignore. Thanks!</t>
   </si>
   <si>
-    <t>mliu@ep.com,spopovic@ep.com</t>
+    <t>&lt;ENTER_YOUR_EMAIL_HERE&gt;</t>
+  </si>
+  <si>
+    <t>email:&lt;INSERT_EMAIL_ADDRESS_HERE&gt;|Scenario $(execution|scenario|name) of $(execution|script|name) has completed.</t>
+  </si>
+  <si>
+    <t>&lt;INSERT_EMAIL_ADDRESS_HERE&gt;</t>
   </si>
 </sst>
 </file>
@@ -427,7 +424,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -459,6 +456,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -469,7 +470,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="66">
     <dxf>
       <font>
         <b val="0"/>
@@ -496,19 +497,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -552,6 +540,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -575,19 +576,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -631,6 +619,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -654,19 +655,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -710,6 +698,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -733,19 +734,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -789,6 +777,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -812,19 +813,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -868,6 +856,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -891,19 +892,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -947,6 +935,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -970,19 +971,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1026,6 +1014,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -1049,19 +1050,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1105,6 +1093,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -1128,19 +1129,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1184,6 +1172,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <u val="none"/>
@@ -1207,19 +1208,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1257,6 +1245,98 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1552,7 +1632,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2994,7 +3074,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -3704,10 +3784,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -7265,10 +7345,10 @@
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -7974,10 +8054,10 @@
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -8683,14 +8763,14 @@
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
@@ -9393,16 +9473,16 @@
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -10105,16 +10185,16 @@
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -10817,16 +10897,16 @@
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -11529,13 +11609,13 @@
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
       <c r="D15"/>
       <c r="E15"/>
@@ -12239,13 +12319,13 @@
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -12949,13 +13029,13 @@
     </row>
     <row r="17" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -13659,10 +13739,10 @@
     </row>
     <row r="18" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
@@ -14367,10 +14447,10 @@
     </row>
     <row r="19" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -15075,10 +15155,10 @@
     </row>
     <row r="20" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -15783,10 +15863,10 @@
     </row>
     <row r="21" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -16491,7 +16571,7 @@
     </row>
     <row r="22" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -16499,7 +16579,7 @@
     </row>
     <row r="23" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -16507,7 +16587,7 @@
     </row>
     <row r="24" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -16515,7 +16595,7 @@
     </row>
     <row r="25" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -16523,7 +16603,7 @@
     </row>
     <row r="26" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -16531,18 +16611,18 @@
     </row>
     <row r="27" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
         <v>52</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="28" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:702" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -17064,24 +17144,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="59" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="65" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="64" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="63" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="57" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="55" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="54" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19189,24 +19269,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19916,24 +19996,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="53" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="59" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="58" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="57" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="51" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="49" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19943,10 +20023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487F2C1F-1995-ED42-8C56-BA026F6A1911}">
-  <dimension ref="A1:AAA200"/>
+  <dimension ref="A1:AAA199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -19959,7 +20039,7 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>4</v>
@@ -19973,10 +20053,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="HA2" s="3" t="s">
         <v>11</v>
@@ -19987,24 +20067,24 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
-      <c r="HA3" s="3" t="s">
+      <c r="HA3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AAA3" s="3" t="s">
+      <c r="AAA3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="HA4" s="6" t="s">
         <v>11</v>
@@ -20015,10 +20095,10 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="HA5" s="6" t="s">
         <v>11</v>
@@ -20042,18 +20122,9 @@
       </c>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="HA7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AAA7" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="HA7" s="6"/>
+      <c r="AAA7" s="7"/>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -20067,8 +20138,6 @@
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="HA10" s="6"/>
-      <c r="AAA10" s="7"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -20636,31 +20705,28 @@
     </row>
     <row r="199" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="47" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="53" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="52" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="51" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20686,10 +20752,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -21399,10 +21465,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -22825,10 +22891,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="HA4" s="6" t="s">
         <v>11</v>
@@ -22839,10 +22905,10 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="HA5" s="6" t="s">
         <v>11</v>
@@ -23467,24 +23533,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="41" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="46" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="45" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="39" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="37" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="36" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23497,7 +23563,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -24936,10 +25002,10 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
+      <c r="B3" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -25649,10 +25715,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -26361,12 +26427,7 @@
       </c>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
@@ -27074,12 +27135,7 @@
       </c>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -27787,12 +27843,7 @@
       </c>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
@@ -28500,12 +28551,8 @@
       </c>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
@@ -29209,12 +29256,8 @@
       <c r="AAA8" s="7"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
@@ -30493,27 +30536,49 @@
       <c r="A200" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="35" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
+  <conditionalFormatting sqref="A1:A2 A4:A1048576">
+    <cfRule type="beginsWith" dxfId="41" priority="7" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="40" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="39" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:AZ2 B4:AZ1048576 C3:AZ3">
+    <cfRule type="expression" dxfId="37" priority="11" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="36" priority="14">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="A3">
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A3,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A3,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A3,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="8">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="6">
+      <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31964,10 +32029,10 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -36115,24 +36180,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="29" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="35" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="34" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="33" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="27" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="24" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36158,10 +36223,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -36871,10 +36936,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -37584,10 +37649,10 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -38297,10 +38362,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -41036,24 +41101,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="23" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="27" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41079,10 +41144,10 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -41792,10 +41857,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -42505,10 +42570,10 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -43218,10 +43283,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -43934,7 +43999,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -45957,24 +46022,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="17" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="21" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45986,8 +46051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12FA983-847F-5043-ABD6-62F9BAA74A18}">
   <dimension ref="A1:AAA200"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -46716,7 +46781,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -47429,7 +47494,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -48139,10 +48204,10 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -48852,10 +48917,10 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -50179,24 +50244,24 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="11" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="15" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>